<commit_message>
Katie - moved over stub fbx loader, updated milestone 1, added fbx objects
</commit_message>
<xml_diff>
--- a/MilestoneOneRubric.xlsx
+++ b/MilestoneOneRubric.xlsx
@@ -29,9 +29,6 @@
     <t>Milestone 1 rubric:</t>
   </si>
   <si>
-    <t>FBX mesh data to binary</t>
-  </si>
-  <si>
     <t>Point Value:</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Build and maintain a repository for the duration of the milestone</t>
   </si>
   <si>
-    <t>Extract FBX mesh data into a binary file</t>
-  </si>
-  <si>
     <t>Should be able to render multiples of a mesh</t>
   </si>
   <si>
@@ -95,13 +89,19 @@
     <t>Loading models</t>
   </si>
   <si>
-    <t>FBX render Binary</t>
-  </si>
-  <si>
-    <t>Render meshes from Binary files</t>
-  </si>
-  <si>
     <t>Team SuperCoolFunYay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBX mesh data </t>
+  </si>
+  <si>
+    <t>Extract FBX mesh data</t>
+  </si>
+  <si>
+    <t>FBX render</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Render meshes </t>
   </si>
 </sst>
 </file>
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -185,9 +185,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,17 +539,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -562,10 +559,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,7 +572,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>35</v>
@@ -583,57 +580,57 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="9">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="6">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="6">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2">
         <v>5</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,13 +639,13 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -656,40 +653,40 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2">
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2">
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="6">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>100</v>

</xml_diff>

<commit_message>
Peter Farber: test commit
</commit_message>
<xml_diff>
--- a/MilestoneOneRubric.xlsx
+++ b/MilestoneOneRubric.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01_SchoolWork\Programming\RTA\Project\RTA_SuperCoolFunYay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MrWiz\Desktop\RTA_SuperCoolFunYay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -185,6 +185,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,7 +530,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +644,7 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="9">
         <v>5</v>
       </c>
       <c r="C14" t="s">
@@ -680,7 +683,7 @@
       <c r="B18" s="6">
         <v>5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Peter Farber: Got fbx loading and rendering.
</commit_message>
<xml_diff>
--- a/MilestoneOneRubric.xlsx
+++ b/MilestoneOneRubric.xlsx
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -185,9 +185,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,7 +527,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +641,7 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="6">
         <v>5</v>
       </c>
       <c r="C14" t="s">
@@ -658,7 +655,7 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="6">
         <v>30</v>
       </c>
       <c r="C16" t="s">
@@ -669,7 +666,7 @@
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="6">
         <v>25</v>
       </c>
       <c r="C17" t="s">

</xml_diff>

<commit_message>
Commit to push new branch
</commit_message>
<xml_diff>
--- a/MilestoneOneRubric.xlsx
+++ b/MilestoneOneRubric.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MrWiz\Desktop\RTA_SuperCoolFunYay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School\Project and Portfolio V\RTAProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -527,14 +527,14 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.28515625" customWidth="1"/>
+    <col min="1" max="1" width="50.25" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" customWidth="1"/>
+    <col min="3" max="3" width="59.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,6 +690,9 @@
       </c>
       <c r="B20" s="2">
         <v>100</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>